<commit_message>
a propos et horaire
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/bd2/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User-Stousignant\Bureau\GitOrganisation\TousignantSimon-BD2.github.io\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448ED297-391E-6845-B5DF-AA00A0BD5CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F14F29-B1D8-4B3B-A7A3-03F6D8575F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1920" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
   <sheets>
     <sheet name="horaire" sheetId="1" r:id="rId1"/>
@@ -907,7 +907,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -977,7 +977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -987,6 +987,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,7 +1006,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -1301,19 +1302,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <cols>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.796875" customWidth="1"/>
     <col min="4" max="4" width="74.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1330,7 +1331,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1338,7 +1339,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4">
-        <v>45525.552083333336</v>
+        <v>45891.427083333336</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -1347,7 +1348,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="109.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="4">
-        <v>45530.34375</v>
+        <v>45894.46875</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>22</v>
@@ -1364,7 +1365,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="78">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1372,7 +1373,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="4">
-        <v>45532.552083333336</v>
+        <v>45898.427083333336</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>35</v>
@@ -1381,15 +1382,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="46.8">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="4">
-        <v>45540.34375</v>
+      <c r="C5" s="5">
+        <v>45901.46875</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>30</v>
@@ -1398,7 +1399,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="43.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1406,7 +1407,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="4">
-        <v>45544.34375</v>
+        <v>45905.427083333336</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>31</v>
@@ -1415,7 +1416,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1423,7 +1424,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="4">
-        <v>45546.552083333336</v>
+        <v>45908.46875</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1432,7 +1433,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1440,13 +1441,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="4">
-        <v>45551.34375</v>
+        <v>45912.427083333336</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="62.4">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="4">
-        <v>45553.552083333336</v>
+        <v>45915.46875</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>32</v>
@@ -1463,7 +1464,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="78">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="4">
-        <v>45558.34375</v>
+        <v>45919.427083333336</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>38</v>
@@ -1480,7 +1481,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1488,7 +1489,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="4">
-        <v>45560.552083333336</v>
+        <v>45922.46875</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
@@ -1497,7 +1498,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1505,7 +1506,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="4">
-        <v>45565.34375</v>
+        <v>45926.427083333336</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -1514,7 +1515,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1522,13 +1523,13 @@
         <v>12</v>
       </c>
       <c r="C13" s="4">
-        <v>45567.552083333336</v>
+        <v>45929.46875</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="31.2">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1536,7 +1537,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="4">
-        <v>45572.34375</v>
+        <v>45933.427083333336</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>41</v>
@@ -1545,7 +1546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="62.4">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1553,7 +1554,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="4">
-        <v>45574.552083333336</v>
+        <v>45936.46875</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -1562,7 +1563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="109.2">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1570,7 +1571,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="4">
-        <v>45586.34375</v>
+        <v>45940.427083333336</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>42</v>
@@ -1579,7 +1580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1587,7 +1588,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="4">
-        <v>45588.552083333336</v>
+        <v>45950.46875</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -1596,7 +1597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="4">
-        <v>45593.34375</v>
+        <v>45954.427083333336</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
@@ -1613,7 +1614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>9</v>
       </c>
@@ -1621,7 +1622,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="4">
-        <v>45595.552083333336</v>
+        <v>45957.46875</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>37</v>
@@ -1630,7 +1631,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1638,14 +1639,14 @@
         <v>19</v>
       </c>
       <c r="C20" s="4">
-        <v>45600.34375</v>
+        <v>45961.427083333336</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1653,13 +1654,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="4">
-        <v>45604.552083333336</v>
+        <v>45968.427083333336</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1667,13 +1668,13 @@
         <v>21</v>
       </c>
       <c r="C22" s="4">
-        <v>45607.34375</v>
+        <v>45971.46875</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1681,13 +1682,13 @@
         <v>22</v>
       </c>
       <c r="C23" s="4">
-        <v>45609.552083333336</v>
+        <v>45975.427083333336</v>
       </c>
       <c r="D23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1695,13 +1696,13 @@
         <v>23</v>
       </c>
       <c r="C24" s="4">
-        <v>45614.34375</v>
+        <v>45978.46875</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>12</v>
       </c>
@@ -1709,13 +1710,13 @@
         <v>24</v>
       </c>
       <c r="C25" s="4">
-        <v>45616.552083333336</v>
+        <v>45982.427083333336</v>
       </c>
       <c r="D25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>13</v>
       </c>
@@ -1723,13 +1724,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="4">
-        <v>45621.34375</v>
+        <v>45985.46875</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1737,13 +1738,13 @@
         <v>26</v>
       </c>
       <c r="C27" s="4">
-        <v>45623.552083333336</v>
+        <v>45989.427083333336</v>
       </c>
       <c r="D27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>14</v>
       </c>
@@ -1751,13 +1752,13 @@
         <v>27</v>
       </c>
       <c r="C28" s="4">
-        <v>45628.34375</v>
+        <v>45992.46875</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>14</v>
       </c>
@@ -1765,13 +1766,13 @@
         <v>28</v>
       </c>
       <c r="C29" s="4">
-        <v>45630.552083333336</v>
+        <v>45996.427083333336</v>
       </c>
       <c r="D29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>15</v>
       </c>
@@ -1779,13 +1780,13 @@
         <v>29</v>
       </c>
       <c r="C30" s="4">
-        <v>45635.34375</v>
+        <v>45999.46875</v>
       </c>
       <c r="D30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>15</v>
       </c>
@@ -1793,11 +1794,14 @@
         <v>30</v>
       </c>
       <c r="C31" s="4">
-        <v>45637.552083333336</v>
+        <v>46003.427083333336</v>
       </c>
       <c r="D31" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="C32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>